<commit_message>
Add downloaded file from Dell ECS
</commit_message>
<xml_diff>
--- a/import/msw_in_region_disposal.xlsx
+++ b/import/msw_in_region_disposal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhathal/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/amandeep_bhathal_gov_bc_ca/Documents/Apps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B19AB092-0EDA-2746-A007-A0B30626F193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AA9F01A-78F2-874A-BF4C-E98EC0D43185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="860" windowWidth="27240" windowHeight="16440" xr2:uid="{AFBB352B-97F1-4B47-BECF-2B0419D74A01}"/>
   </bookViews>
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="128">
+  <si>
+    <t>"MSW In-Region Disposal: Jan 1, 2022 - Dec 31, 2022"</t>
+  </si>
   <si>
     <t>Member</t>
   </si>
@@ -1261,181 +1264,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF8375-3BDB-004A-8564-E6E1A96902AB}">
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="43.5" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2">
-        <v>2100871</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>524</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>15256</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>2100871</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>5634</v>
+        <v>524</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3">
-        <v>7267.5</v>
+        <v>15256</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>2100871</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>2100877</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>12659</v>
+        <v>5634</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4">
-        <v>180004</v>
+        <v>7267.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>2100877</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
-        <v>2100881</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>3132</v>
+        <v>12659</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G5">
-        <v>17595</v>
+        <v>180004</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>2100881</v>
       </c>
       <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
       <c r="E6">
-        <v>4533</v>
+        <v>3132</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G6">
-        <v>325</v>
+        <v>17595</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>2100881</v>
       </c>
       <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>4533</v>
+      </c>
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>4535</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
       <c r="G7">
-        <v>50</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>2100881</v>
@@ -1444,21 +1424,21 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>4536</v>
+        <v>4535</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8">
-        <v>85</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>2100881</v>
@@ -1467,21 +1447,21 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>4994</v>
+        <v>4536</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G9">
-        <v>7968</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>2100881</v>
@@ -1490,21 +1470,21 @@
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>5776</v>
+        <v>4994</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G10">
-        <v>1200</v>
+        <v>7968</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>2100881</v>
@@ -1513,21 +1493,21 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11">
-        <v>6313</v>
+        <v>5776</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11">
-        <v>20</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>2100881</v>
@@ -1536,21 +1516,21 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>6510</v>
+        <v>6313</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12">
-        <v>350</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>2100881</v>
@@ -1559,21 +1539,21 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13">
-        <v>6922</v>
+        <v>6510</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G13">
-        <v>25</v>
+        <v>350</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>2100881</v>
@@ -1582,21 +1562,21 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14">
-        <v>7200</v>
+        <v>6922</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>2100881</v>
@@ -1605,21 +1585,21 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>7644</v>
+        <v>7200</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>2100881</v>
@@ -1628,21 +1608,21 @@
         <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>10953</v>
+        <v>7644</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16">
-        <v>115</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>2100881</v>
@@ -1651,21 +1631,21 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E17">
-        <v>11071</v>
+        <v>10953</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G17">
-        <v>225</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>2100881</v>
@@ -1674,21 +1654,21 @@
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E18">
-        <v>16556</v>
+        <v>11071</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G18">
-        <v>10693</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>2100881</v>
@@ -1697,21 +1677,21 @@
         <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19">
-        <v>17920</v>
+        <v>16556</v>
       </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>495</v>
+        <v>10693</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20">
         <v>2100881</v>
@@ -1720,44 +1700,44 @@
         <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E20">
-        <v>103019</v>
+        <v>17920</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G20">
-        <v>2658</v>
+        <v>495</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>2100881</v>
+      </c>
+      <c r="C21" t="s">
         <v>33</v>
       </c>
-      <c r="B21">
-        <v>2100891</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E21">
-        <v>4223</v>
+        <v>103019</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G21">
-        <v>1576</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22">
         <v>2100891</v>
@@ -1766,18 +1746,21 @@
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E22">
-        <v>10611</v>
+        <v>4223</v>
       </c>
       <c r="F22" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="G22">
+        <v>1576</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>2100891</v>
@@ -1786,58 +1769,55 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E23">
-        <v>18186</v>
+        <v>10611</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>2100891</v>
       </c>
       <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
         <v>38</v>
       </c>
-      <c r="D24" t="s">
-        <v>37</v>
+      <c r="E24">
+        <v>18186</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>2100891</v>
+      </c>
+      <c r="C25" t="s">
         <v>39</v>
       </c>
-      <c r="B25">
-        <v>2100899</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
       <c r="D25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25">
-        <v>514</v>
+        <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25">
-        <v>3218</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>2100899</v>
@@ -1846,21 +1826,21 @@
         <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E26">
-        <v>5479</v>
+        <v>514</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G26">
-        <v>31232</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27">
         <v>2100899</v>
@@ -1869,21 +1849,21 @@
         <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E27">
-        <v>15821</v>
+        <v>5479</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G27">
-        <v>7414</v>
+        <v>31232</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>2100899</v>
@@ -1892,44 +1872,44 @@
         <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E28">
-        <v>17006</v>
+        <v>15821</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G28">
-        <v>5331</v>
+        <v>7414</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>2100899</v>
+      </c>
+      <c r="C29" t="s">
         <v>44</v>
       </c>
-      <c r="B29">
-        <v>2100901</v>
-      </c>
-      <c r="C29" t="s">
-        <v>45</v>
-      </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E29">
-        <v>2401</v>
+        <v>17006</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G29">
-        <v>2201</v>
+        <v>5331</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>2100901</v>
@@ -1938,18 +1918,21 @@
         <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E30">
-        <v>3825</v>
+        <v>2401</v>
       </c>
       <c r="F30" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="G30">
+        <v>2201</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B31">
         <v>2100901</v>
@@ -1958,21 +1941,18 @@
         <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E31">
-        <v>4278</v>
+        <v>3825</v>
       </c>
       <c r="F31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31">
-        <v>650</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B32">
         <v>2100901</v>
@@ -1981,21 +1961,21 @@
         <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E32">
-        <v>5050</v>
+        <v>4278</v>
       </c>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G32">
-        <v>61944</v>
+        <v>650</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B33">
         <v>2100901</v>
@@ -2004,44 +1984,44 @@
         <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E33">
-        <v>7496</v>
+        <v>5050</v>
       </c>
       <c r="F33" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G33">
-        <v>493</v>
+        <v>61944</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <v>2100901</v>
+      </c>
+      <c r="C34" t="s">
         <v>50</v>
       </c>
-      <c r="B34">
-        <v>2100927</v>
-      </c>
-      <c r="C34" t="s">
-        <v>51</v>
-      </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>1697</v>
+        <v>7496</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G34">
-        <v>74416.7</v>
+        <v>493</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35">
         <v>2100927</v>
@@ -2050,18 +2030,21 @@
         <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E35">
-        <v>6424</v>
+        <v>1697</v>
       </c>
       <c r="F35" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="G35">
+        <v>74416.7</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B36">
         <v>2100927</v>
@@ -2070,21 +2053,18 @@
         <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E36">
-        <v>100206</v>
+        <v>6424</v>
       </c>
       <c r="F36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36">
-        <v>539</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37">
         <v>2100927</v>
@@ -2092,33 +2072,33 @@
       <c r="C37" t="s">
         <v>54</v>
       </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>100206</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37">
+        <v>539</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38">
+        <v>2100927</v>
+      </c>
+      <c r="C38" t="s">
         <v>55</v>
-      </c>
-      <c r="B38">
-        <v>2100935</v>
-      </c>
-      <c r="C38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38">
-        <v>101798</v>
-      </c>
-      <c r="F38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38">
-        <v>86882.58</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B39">
         <v>2100935</v>
@@ -2127,21 +2107,21 @@
         <v>57</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E39">
-        <v>101804</v>
+        <v>101798</v>
       </c>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G39">
-        <v>383.44</v>
+        <v>86882.58</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B40">
         <v>2100935</v>
@@ -2150,21 +2130,21 @@
         <v>58</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E40">
-        <v>105058</v>
+        <v>101804</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G40">
-        <v>13875.49</v>
+        <v>383.44</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B41">
         <v>2100935</v>
@@ -2173,41 +2153,41 @@
         <v>59</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="E41">
+        <v>105058</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G41">
-        <v>-82000</v>
+        <v>13875.49</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42">
+        <v>2100935</v>
+      </c>
+      <c r="C42" t="s">
         <v>60</v>
       </c>
-      <c r="B42">
-        <v>2100945</v>
-      </c>
-      <c r="C42" t="s">
-        <v>61</v>
-      </c>
       <c r="D42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42">
-        <v>1611</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G42">
-        <v>683496</v>
+        <v>-82000</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B43">
         <v>2100945</v>
@@ -2216,21 +2196,21 @@
         <v>62</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E43">
-        <v>107051</v>
+        <v>1611</v>
       </c>
       <c r="F43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G43">
-        <v>233052</v>
+        <v>683496</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B44">
         <v>2100945</v>
@@ -2239,41 +2219,41 @@
         <v>63</v>
       </c>
       <c r="D44" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="E44">
+        <v>107051</v>
       </c>
       <c r="F44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G44">
-        <v>185143.01</v>
+        <v>233052</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45">
+        <v>2100945</v>
+      </c>
+      <c r="C45" t="s">
         <v>64</v>
       </c>
-      <c r="B45">
-        <v>2101029</v>
-      </c>
-      <c r="C45" t="s">
-        <v>65</v>
-      </c>
       <c r="D45" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45">
-        <v>7150</v>
+        <v>38</v>
       </c>
       <c r="F45" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G45">
-        <v>1860</v>
+        <v>185143.01</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B46">
         <v>2101029</v>
@@ -2282,67 +2262,67 @@
         <v>66</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E46">
-        <v>7988</v>
+        <v>7150</v>
       </c>
       <c r="F46" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G46">
-        <v>11797</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47">
+        <v>2101029</v>
+      </c>
+      <c r="C47" t="s">
         <v>67</v>
       </c>
-      <c r="B47">
-        <v>2101035</v>
-      </c>
-      <c r="C47" t="s">
-        <v>68</v>
-      </c>
       <c r="D47" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E47">
-        <v>16960</v>
+        <v>7988</v>
       </c>
       <c r="F47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G47">
-        <v>1845.48</v>
+        <v>11797</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48">
+        <v>2101035</v>
+      </c>
+      <c r="C48" t="s">
         <v>69</v>
       </c>
-      <c r="B48">
-        <v>2101047</v>
-      </c>
-      <c r="C48" t="s">
-        <v>70</v>
-      </c>
       <c r="D48" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E48">
-        <v>2896</v>
+        <v>16960</v>
       </c>
       <c r="F48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G48">
-        <v>5406.9</v>
+        <v>1845.48</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B49">
         <v>2101047</v>
@@ -2351,21 +2331,21 @@
         <v>71</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E49">
-        <v>17529</v>
+        <v>2896</v>
       </c>
       <c r="F49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G49">
-        <v>14613.69</v>
+        <v>5406.9</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B50">
         <v>2101047</v>
@@ -2374,44 +2354,44 @@
         <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E50">
-        <v>106160</v>
+        <v>17529</v>
       </c>
       <c r="F50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G50">
-        <v>31862.27</v>
+        <v>14613.69</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51">
+        <v>2101047</v>
+      </c>
+      <c r="C51" t="s">
         <v>73</v>
       </c>
-      <c r="B51">
-        <v>2101077</v>
-      </c>
-      <c r="C51" t="s">
-        <v>74</v>
-      </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E51">
-        <v>4612</v>
+        <v>106160</v>
       </c>
       <c r="F51" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G51">
-        <v>490</v>
+        <v>31862.27</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B52">
         <v>2101077</v>
@@ -2420,21 +2400,21 @@
         <v>75</v>
       </c>
       <c r="D52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E52">
-        <v>5511</v>
+        <v>4612</v>
       </c>
       <c r="F52" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G52">
-        <v>226</v>
+        <v>490</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B53">
         <v>2101077</v>
@@ -2443,21 +2423,21 @@
         <v>76</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E53">
-        <v>15681</v>
+        <v>5511</v>
       </c>
       <c r="F53" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G53">
-        <v>5095</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B54">
         <v>2101077</v>
@@ -2466,21 +2446,21 @@
         <v>77</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E54">
-        <v>17226</v>
+        <v>15681</v>
       </c>
       <c r="F54" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G54">
-        <v>4956</v>
+        <v>5095</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B55">
         <v>2101077</v>
@@ -2489,21 +2469,21 @@
         <v>78</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E55">
-        <v>17227</v>
+        <v>17226</v>
       </c>
       <c r="F55" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G55">
-        <v>21287</v>
+        <v>4956</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B56">
         <v>2101077</v>
@@ -2512,18 +2492,21 @@
         <v>79</v>
       </c>
       <c r="D56" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E56">
-        <v>3608</v>
+        <v>17227</v>
       </c>
       <c r="F56" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="G56">
+        <v>21287</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B57">
         <v>2101077</v>
@@ -2532,18 +2515,18 @@
         <v>80</v>
       </c>
       <c r="D57" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E57">
-        <v>5425</v>
+        <v>3608</v>
       </c>
       <c r="F57" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B58">
         <v>2101077</v>
@@ -2552,41 +2535,38 @@
         <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E58">
-        <v>11936</v>
+        <v>5425</v>
       </c>
       <c r="F58" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59">
+        <v>2101077</v>
+      </c>
+      <c r="C59" t="s">
         <v>82</v>
       </c>
-      <c r="B59">
-        <v>2101081</v>
-      </c>
-      <c r="C59" t="s">
-        <v>83</v>
-      </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E59">
-        <v>1917</v>
+        <v>11936</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59">
-        <v>10602</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B60">
         <v>2101081</v>
@@ -2595,21 +2575,21 @@
         <v>84</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E60">
-        <v>15290</v>
+        <v>1917</v>
       </c>
       <c r="F60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G60">
-        <v>6866.19</v>
+        <v>10602</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B61">
         <v>2101081</v>
@@ -2618,44 +2598,44 @@
         <v>85</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E61">
-        <v>15294</v>
+        <v>15290</v>
       </c>
       <c r="F61" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G61">
-        <v>1062.18</v>
+        <v>6866.19</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62">
+        <v>2101081</v>
+      </c>
+      <c r="C62" t="s">
         <v>86</v>
       </c>
-      <c r="B62">
-        <v>2101099</v>
-      </c>
-      <c r="C62" t="s">
-        <v>87</v>
-      </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E62">
-        <v>7912</v>
+        <v>15294</v>
       </c>
       <c r="F62" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G62">
-        <v>20</v>
+        <v>1062.18</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B63">
         <v>2101099</v>
@@ -2664,21 +2644,21 @@
         <v>88</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E63">
-        <v>8856</v>
+        <v>7912</v>
       </c>
       <c r="F63" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G63">
-        <v>15052</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B64">
         <v>2101099</v>
@@ -2687,44 +2667,44 @@
         <v>89</v>
       </c>
       <c r="D64" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E64">
-        <v>17686</v>
+        <v>8856</v>
       </c>
       <c r="F64" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G64">
-        <v>11163</v>
+        <v>15052</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65">
+        <v>2101099</v>
+      </c>
+      <c r="C65" t="s">
         <v>90</v>
       </c>
-      <c r="B65">
-        <v>2101101</v>
-      </c>
-      <c r="C65" t="s">
-        <v>91</v>
-      </c>
       <c r="D65" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E65">
-        <v>16521</v>
+        <v>17686</v>
       </c>
       <c r="F65" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G65">
-        <v>1677.6</v>
+        <v>11163</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B66">
         <v>2101101</v>
@@ -2733,21 +2713,21 @@
         <v>92</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E66">
-        <v>16913</v>
+        <v>16521</v>
       </c>
       <c r="F66" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G66">
-        <v>7079.3</v>
+        <v>1677.6</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B67">
         <v>2101101</v>
@@ -2756,67 +2736,67 @@
         <v>93</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E67">
-        <v>17126</v>
+        <v>16913</v>
       </c>
       <c r="F67" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G67">
-        <v>21163.200000000001</v>
+        <v>7079.3</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68">
+        <v>2101101</v>
+      </c>
+      <c r="C68" t="s">
         <v>94</v>
       </c>
-      <c r="B68">
-        <v>2101105</v>
-      </c>
-      <c r="C68" t="s">
-        <v>95</v>
-      </c>
       <c r="D68" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E68">
-        <v>12218</v>
+        <v>17126</v>
       </c>
       <c r="F68" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G68">
-        <v>146833</v>
+        <v>21163.200000000001</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>95</v>
+      </c>
+      <c r="B69">
+        <v>2101105</v>
+      </c>
+      <c r="C69" t="s">
         <v>96</v>
       </c>
-      <c r="B69">
-        <v>2101119</v>
-      </c>
-      <c r="C69" t="s">
-        <v>97</v>
-      </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E69">
-        <v>15962</v>
+        <v>12218</v>
       </c>
       <c r="F69" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G69">
-        <v>35267.75</v>
+        <v>146833</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B70">
         <v>2101119</v>
@@ -2825,21 +2805,21 @@
         <v>98</v>
       </c>
       <c r="D70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E70">
-        <v>100134</v>
+        <v>15962</v>
       </c>
       <c r="F70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G70">
-        <v>13363.72</v>
+        <v>35267.75</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B71">
         <v>2101119</v>
@@ -2848,90 +2828,90 @@
         <v>99</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E71">
-        <v>107745</v>
+        <v>100134</v>
       </c>
       <c r="F71" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G71">
-        <v>1394.36</v>
+        <v>13363.72</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72">
+        <v>2101119</v>
+      </c>
+      <c r="C72" t="s">
         <v>100</v>
       </c>
-      <c r="B72">
-        <v>2101123</v>
-      </c>
-      <c r="C72" t="s">
-        <v>101</v>
-      </c>
       <c r="D72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E72">
-        <v>8490</v>
+        <v>107745</v>
       </c>
       <c r="F72" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G72">
-        <v>7762</v>
+        <v>1394.36</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>101</v>
+      </c>
+      <c r="B73">
+        <v>2101123</v>
+      </c>
+      <c r="C73" t="s">
         <v>102</v>
       </c>
-      <c r="B73">
-        <v>2101127</v>
-      </c>
-      <c r="C73" t="s">
-        <v>103</v>
-      </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E73">
-        <v>1714</v>
+        <v>8490</v>
       </c>
       <c r="F73" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G73">
-        <v>75553</v>
+        <v>7762</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>103</v>
+      </c>
+      <c r="B74">
+        <v>2101127</v>
+      </c>
+      <c r="C74" t="s">
         <v>104</v>
       </c>
-      <c r="B74">
-        <v>2101139</v>
-      </c>
-      <c r="C74" t="s">
-        <v>105</v>
-      </c>
       <c r="D74" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E74">
-        <v>15282</v>
+        <v>1714</v>
       </c>
       <c r="F74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G74">
-        <v>2364</v>
+        <v>75553</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B75">
         <v>2101139</v>
@@ -2940,21 +2920,21 @@
         <v>106</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E75">
-        <v>15284</v>
+        <v>15282</v>
       </c>
       <c r="F75" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G75">
-        <v>14189</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B76">
         <v>2101139</v>
@@ -2963,38 +2943,44 @@
         <v>107</v>
       </c>
       <c r="D76" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E76">
-        <v>15286</v>
+        <v>15284</v>
       </c>
       <c r="F76" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G76">
-        <v>29595</v>
+        <v>14189</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77">
+        <v>2101139</v>
+      </c>
+      <c r="C77" t="s">
         <v>108</v>
       </c>
-      <c r="B77">
-        <v>2101141</v>
-      </c>
-      <c r="C77" t="s">
-        <v>109</v>
+      <c r="D77" t="s">
+        <v>10</v>
       </c>
       <c r="E77">
-        <v>15273</v>
+        <v>15286</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
       </c>
       <c r="G77">
-        <v>4045</v>
+        <v>29595</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B78">
         <v>2101141</v>
@@ -3002,22 +2988,16 @@
       <c r="C78" t="s">
         <v>110</v>
       </c>
-      <c r="D78" t="s">
-        <v>9</v>
-      </c>
       <c r="E78">
-        <v>15274</v>
-      </c>
-      <c r="F78" t="s">
-        <v>10</v>
+        <v>15273</v>
       </c>
       <c r="G78">
-        <v>27061</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B79">
         <v>2101141</v>
@@ -3025,16 +3005,22 @@
       <c r="C79" t="s">
         <v>111</v>
       </c>
+      <c r="D79" t="s">
+        <v>10</v>
+      </c>
       <c r="E79">
-        <v>15275</v>
+        <v>15274</v>
+      </c>
+      <c r="F79" t="s">
+        <v>11</v>
       </c>
       <c r="G79">
-        <v>5581</v>
+        <v>27061</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B80">
         <v>2101141</v>
@@ -3043,15 +3029,15 @@
         <v>112</v>
       </c>
       <c r="E80">
-        <v>15276</v>
+        <v>15275</v>
       </c>
       <c r="G80">
-        <v>4271</v>
+        <v>5581</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B81">
         <v>2101141</v>
@@ -3059,22 +3045,16 @@
       <c r="C81" t="s">
         <v>113</v>
       </c>
-      <c r="D81" t="s">
-        <v>9</v>
-      </c>
       <c r="E81">
-        <v>15279</v>
-      </c>
-      <c r="F81" t="s">
-        <v>10</v>
+        <v>15276</v>
       </c>
       <c r="G81">
-        <v>3987</v>
+        <v>4271</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B82">
         <v>2101141</v>
@@ -3083,44 +3063,44 @@
         <v>114</v>
       </c>
       <c r="D82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E82">
-        <v>15280</v>
+        <v>15279</v>
       </c>
       <c r="F82" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G82">
-        <v>7982</v>
+        <v>3987</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83">
+        <v>2101141</v>
+      </c>
+      <c r="C83" t="s">
         <v>115</v>
       </c>
-      <c r="B83">
-        <v>2101145</v>
-      </c>
-      <c r="C83" t="s">
-        <v>116</v>
-      </c>
       <c r="D83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E83">
-        <v>5042</v>
+        <v>15280</v>
       </c>
       <c r="F83" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G83">
-        <v>2893</v>
+        <v>7982</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B84">
         <v>2101145</v>
@@ -3129,67 +3109,67 @@
         <v>117</v>
       </c>
       <c r="D84" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E84">
-        <v>106063</v>
+        <v>5042</v>
       </c>
       <c r="F84" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G84">
-        <v>11940</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>116</v>
+      </c>
+      <c r="B85">
+        <v>2101145</v>
+      </c>
+      <c r="C85" t="s">
         <v>118</v>
       </c>
-      <c r="B85">
-        <v>2101147</v>
-      </c>
-      <c r="C85" t="s">
-        <v>119</v>
-      </c>
       <c r="D85" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E85">
-        <v>106060</v>
+        <v>106063</v>
       </c>
       <c r="F85" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G85">
-        <v>12239</v>
+        <v>11940</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>119</v>
+      </c>
+      <c r="B86">
+        <v>2101147</v>
+      </c>
+      <c r="C86" t="s">
         <v>120</v>
       </c>
-      <c r="B86">
-        <v>2101149</v>
-      </c>
-      <c r="C86" t="s">
-        <v>121</v>
-      </c>
       <c r="D86" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E86">
-        <v>3328</v>
+        <v>106060</v>
       </c>
       <c r="F86" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G86">
-        <v>61762</v>
+        <v>12239</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B87">
         <v>2101149</v>
@@ -3198,21 +3178,21 @@
         <v>122</v>
       </c>
       <c r="D87" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E87">
-        <v>3447</v>
+        <v>3328</v>
       </c>
       <c r="F87" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G87">
-        <v>6661</v>
+        <v>61762</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B88">
         <v>2101149</v>
@@ -3221,21 +3201,21 @@
         <v>123</v>
       </c>
       <c r="D88" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E88">
-        <v>4465</v>
+        <v>3447</v>
       </c>
       <c r="F88" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G88">
-        <v>13245</v>
+        <v>6661</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B89">
         <v>2101149</v>
@@ -3244,21 +3224,21 @@
         <v>124</v>
       </c>
       <c r="D89" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E89">
-        <v>4778</v>
+        <v>4465</v>
       </c>
       <c r="F89" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G89">
-        <v>2800</v>
+        <v>13245</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B90">
         <v>2101149</v>
@@ -3267,21 +3247,21 @@
         <v>125</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E90">
-        <v>5910</v>
+        <v>4778</v>
       </c>
       <c r="F90" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G90">
-        <v>10703</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B91">
         <v>2101149</v>
@@ -3290,20 +3270,43 @@
         <v>126</v>
       </c>
       <c r="D91" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E91">
+        <v>5910</v>
+      </c>
+      <c r="F91" t="s">
+        <v>11</v>
+      </c>
+      <c r="G91">
+        <v>10703</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>121</v>
+      </c>
+      <c r="B92">
+        <v>2101149</v>
+      </c>
+      <c r="C92" t="s">
+        <v>127</v>
+      </c>
+      <c r="D92" t="s">
+        <v>38</v>
+      </c>
+      <c r="E92">
         <v>107189</v>
       </c>
-      <c r="F91" t="s">
-        <v>10</v>
-      </c>
-      <c r="G91">
+      <c r="F92" t="s">
+        <v>11</v>
+      </c>
+      <c r="G92">
         <v>2884</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G92">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G93">
         <v>2232849.36</v>
       </c>
     </row>

</xml_diff>